<commit_message>
exercise done - po -am
hands on exercise - am - day1 - potential outcome
</commit_message>
<xml_diff>
--- a/Exercises/Perfect_Doctor.xlsx
+++ b/Exercises/Perfect_Doctor.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott_cunningham/Documents/Mixtape_tracks/Assignments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgiar-my.sharepoint.com/personal/a_mitra_cgiar_org1/Documents/Documents/Github/Causal-Inference/Exercises/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673C66E6-8AA4-6B4D-95EB-BCF49F3E42BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:1_{673C66E6-8AA4-6B4D-95EB-BCF49F3E42BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{85587D1F-614D-46A8-9C80-226F39B26F24}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="1060" windowWidth="24840" windowHeight="25820" activeTab="1" xr2:uid="{083BD555-0A53-1B4B-AE70-5F7A5361EDB7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{083BD555-0A53-1B4B-AE70-5F7A5361EDB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>Person</t>
   </si>
@@ -120,6 +122,12 @@
   </si>
   <si>
     <t>Avg(Y |D=1) - Avg(Y |D=0)</t>
+  </si>
+  <si>
+    <t>ATT - ATU</t>
+  </si>
+  <si>
+    <t>(1 - PI) * (ATT -ATU)</t>
   </si>
 </sst>
 </file>
@@ -143,7 +151,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,6 +179,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -258,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -268,13 +282,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,15 +607,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72EDE92-11F1-504D-AA85-77E1FD099BAB}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection sqref="A1:F13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -613,11 +631,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -634,12 +652,12 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2">
-        <f>E2*C2+(1-E2)*B2</f>
+      <c r="F2" s="13">
+        <f>E2*C2 + (1-E2)*B2</f>
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -656,12 +674,12 @@
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F13" si="1">E3*C3+(1-E3)*B3</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F3" s="13">
+        <f>E3*C3 + (1-E3)*B3</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -678,144 +696,144 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="13">
+        <f t="shared" ref="F4:F13" si="1">E4*C4 + (1-E4)*B4</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6">
+        <v>8</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="13">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="5">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="13">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="5">
+        <v>10</v>
+      </c>
+      <c r="C7" s="6">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="13">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="5">
-        <v>7</v>
-      </c>
-      <c r="C5" s="6">
-        <v>8</v>
-      </c>
-      <c r="D5" s="7">
-        <f t="shared" si="0"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="5">
+        <v>2</v>
+      </c>
+      <c r="C8" s="6">
+        <v>2</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="13">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="5">
+        <v>4</v>
+      </c>
+      <c r="C9" s="6">
         <v>1</v>
       </c>
-      <c r="E5">
+      <c r="D9" s="7">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="13">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="5">
+        <v>2</v>
+      </c>
+      <c r="C10" s="6">
+        <v>10</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E10">
         <v>1</v>
       </c>
-      <c r="F5">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="5">
-        <v>8</v>
-      </c>
-      <c r="C6" s="6">
-        <v>5</v>
-      </c>
-      <c r="D6" s="7">
-        <f t="shared" si="0"/>
-        <v>-3</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="5">
-        <v>10</v>
-      </c>
-      <c r="C7" s="6">
-        <v>6</v>
-      </c>
-      <c r="D7" s="7">
-        <f t="shared" si="0"/>
-        <v>-4</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
+      <c r="F10" s="13">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="5">
-        <v>2</v>
-      </c>
-      <c r="C8" s="6">
-        <v>2</v>
-      </c>
-      <c r="D8" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="5">
-        <v>4</v>
-      </c>
-      <c r="C9" s="6">
-        <v>1</v>
-      </c>
-      <c r="D9" s="7">
-        <f t="shared" si="0"/>
-        <v>-3</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="5">
-        <v>2</v>
-      </c>
-      <c r="C10" s="6">
-        <v>10</v>
-      </c>
-      <c r="D10" s="7">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -832,12 +850,12 @@
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="13">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -854,12 +872,12 @@
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="13">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -876,12 +894,12 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="13">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>18</v>
       </c>
@@ -889,76 +907,90 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="9">
-        <f>AVERAGE(F3,F5,F10:F11,F13) - AVERAGE(F2,F4,F6:F9,F12)</f>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="17">
+        <f>AVERAGE(F3,F5,F10,F11,F13) - AVERAGE(F2,F4,F6:F9,F12)</f>
         <v>1.3428571428571425</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
+    <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="10" t="s">
         <v>23</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
-        <f>AVERAGE(B3,B5,B10:B11,B13)</f>
+      <c r="H19" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="14">
+        <f>AVERAGE(B3,B5,B10,B11,B13)</f>
         <v>3</v>
       </c>
-      <c r="B20" s="13">
+      <c r="B20" s="15">
         <f>AVERAGE(B2,B4,B6:B9,B12)</f>
         <v>6.8571428571428568</v>
       </c>
-      <c r="C20" s="12">
-        <f>SUM(E2:E13)/COUNT(E2:E13)</f>
+      <c r="C20" s="14">
+        <f>5/12</f>
         <v>0.41666666666666669</v>
       </c>
-      <c r="D20" s="15">
-        <f>AVERAGE(D3,D5,D10:D11,D13)</f>
+      <c r="D20" s="16">
+        <f>AVERAGE(D13,D11,D10,D5,D3)</f>
         <v>5.2</v>
       </c>
-      <c r="E20" s="13">
-        <f>AVERAGE(D2,D4,D6:D9,D12)</f>
+      <c r="E20" s="15">
+        <f>AVERAGE(D12,D7:D9,D6,D4,D2)</f>
         <v>-3.2857142857142856</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="17">
         <f>AVERAGE(D2:D13)</f>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H20" s="19">
+        <f>D20-E20</f>
+        <v>8.4857142857142858</v>
+      </c>
+      <c r="I20" s="19">
+        <f>(1 - C20) * H20</f>
+        <v>4.9499999999999993</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="19">
         <f>F20+ A20-B20+(1-C20)*(D20-E20)</f>
         <v>1.3428571428571425</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -972,13 +1004,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{658F0CAF-38BA-064D-B720-EB93DBD0638C}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -998,7 +1030,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1008,9 +1040,12 @@
       <c r="C2" s="6">
         <v>10</v>
       </c>
-      <c r="D2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D2" s="7">
+        <f>C2-B2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1020,9 +1055,12 @@
       <c r="C3" s="6">
         <v>15</v>
       </c>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:D13" si="0">C3-B3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1032,9 +1070,12 @@
       <c r="C4" s="6">
         <v>12</v>
       </c>
-      <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D4" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1044,9 +1085,12 @@
       <c r="C5" s="6">
         <v>11</v>
       </c>
-      <c r="D5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D5" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1056,9 +1100,12 @@
       <c r="C6" s="6">
         <v>9</v>
       </c>
-      <c r="D6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1068,9 +1115,12 @@
       <c r="C7" s="6">
         <v>11</v>
       </c>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1080,9 +1130,12 @@
       <c r="C8" s="6">
         <v>7</v>
       </c>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1092,9 +1145,12 @@
       <c r="C9" s="6">
         <v>11</v>
       </c>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D9" s="7">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1104,9 +1160,12 @@
       <c r="C10" s="6">
         <v>6</v>
       </c>
-      <c r="D10" s="7"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D10" s="7">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1116,9 +1175,12 @@
       <c r="C11" s="6">
         <v>9</v>
       </c>
-      <c r="D11" s="7"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D11" s="7">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1128,9 +1190,12 @@
       <c r="C12" s="6">
         <v>13</v>
       </c>
-      <c r="D12" s="7"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D12" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1140,7 +1205,10 @@
       <c r="C13" s="6">
         <v>15</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>